<commit_message>
changing document, table attributes to lowerCamelCase
</commit_message>
<xml_diff>
--- a/examples/biochemical_models/data.xlsx
+++ b/examples/biochemical_models/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="4" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="6840" windowWidth="20295"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="20295" windowHeight="6840" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!_Table of contents" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,10 +16,10 @@
     <externalReference xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
   </externalReferences>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'!!_Table of contents'!$A$2:$C$6</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'!!_Schema'!$A$2:$G$19</definedName>
-    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'!!Compound'!$A$2:$E$7</definedName>
-    <definedName hidden="1" localSheetId="4" name="_xlnm._FilterDatabase">'!!Reaction'!$A$2:$G$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!_Table of contents'!$A$2:$C$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'!!_Schema'!$A$2:$G$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'!!Compound'!$A$2:$E$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'!!Reaction'!$A$2:$G$4</definedName>
   </definedNames>
   <calcPr calcId="144525" fullCalcOnLoad="1"/>
 </workbook>
@@ -28,9 +28,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" numFmtId="164"/>
-    <numFmt formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ " numFmtId="165"/>
-    <numFmt formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ " numFmtId="166"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -519,217 +519,217 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="28" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="31" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="13" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="32" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="33" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="23" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="34" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="27" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="26" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="29" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="25" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="24" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="11" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="19" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="12" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="21" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="20" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="22" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="18" fontId="20" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="30" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="9" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="17" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="0" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="10" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="16" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="15" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="14" fontId="19" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="13" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="10" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="5" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="13" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="21" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="22" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="165">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="7" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="42">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="166">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="6" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="8" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="52" name="60% - Accent6" xfId="1"/>
-    <cellStyle builtinId="51" name="40% - Accent6" xfId="2"/>
-    <cellStyle builtinId="48" name="60% - Accent5" xfId="3"/>
-    <cellStyle builtinId="49" name="Accent6" xfId="4"/>
-    <cellStyle builtinId="47" name="40% - Accent5" xfId="5"/>
-    <cellStyle builtinId="46" name="20% - Accent5" xfId="6"/>
-    <cellStyle builtinId="44" name="60% - Accent4" xfId="7"/>
-    <cellStyle builtinId="45" name="Accent5" xfId="8"/>
-    <cellStyle builtinId="43" name="40% - Accent4" xfId="9"/>
-    <cellStyle builtinId="41" name="Accent4" xfId="10"/>
-    <cellStyle builtinId="24" name="Linked Cell" xfId="11"/>
-    <cellStyle builtinId="39" name="40% - Accent3" xfId="12"/>
-    <cellStyle builtinId="36" name="60% - Accent2" xfId="13"/>
-    <cellStyle builtinId="37" name="Accent3" xfId="14"/>
-    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
-    <cellStyle builtinId="34" name="20% - Accent2" xfId="16"/>
-    <cellStyle builtinId="33" name="Accent2" xfId="17"/>
-    <cellStyle builtinId="31" name="40% - Accent1" xfId="18"/>
-    <cellStyle builtinId="30" name="20% - Accent1" xfId="19"/>
-    <cellStyle builtinId="29" name="Accent1" xfId="20"/>
-    <cellStyle builtinId="28" name="Neutral" xfId="21"/>
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="22"/>
-    <cellStyle builtinId="27" name="Bad" xfId="23"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="24"/>
-    <cellStyle builtinId="25" name="Total" xfId="25"/>
-    <cellStyle builtinId="21" name="Output" xfId="26"/>
-    <cellStyle builtinId="4" name="Currency" xfId="27"/>
-    <cellStyle builtinId="38" name="20% - Accent3" xfId="28"/>
-    <cellStyle builtinId="10" name="Note" xfId="29"/>
-    <cellStyle builtinId="20" name="Input" xfId="30"/>
-    <cellStyle builtinId="19" name="Heading 4" xfId="31"/>
-    <cellStyle builtinId="22" name="Calculation" xfId="32"/>
-    <cellStyle builtinId="26" name="Good" xfId="33"/>
-    <cellStyle builtinId="18" name="Heading 3" xfId="34"/>
-    <cellStyle builtinId="53" name="CExplanatory Text" xfId="35"/>
-    <cellStyle builtinId="16" name="Heading 1" xfId="36"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="37"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="38"/>
-    <cellStyle builtinId="15" name="Title" xfId="39"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="40"/>
-    <cellStyle builtinId="11" name="Warning Text" xfId="41"/>
-    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="42"/>
-    <cellStyle builtinId="17" name="Heading 2" xfId="43"/>
-    <cellStyle builtinId="3" name="Comma" xfId="44"/>
-    <cellStyle builtinId="23" name="Check Cell" xfId="45"/>
-    <cellStyle builtinId="40" name="60% - Accent3" xfId="46"/>
-    <cellStyle builtinId="5" name="Percent" xfId="47"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="48"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -739,12 +739,12 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Select a value from "Model:1" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Identifier
 Enter a string.
@@ -752,20 +752,20 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Name
 Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Select "True" or "False".</t>
       </text>
@@ -780,7 +780,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Identifier
 Enter a string.
@@ -788,7 +788,7 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A3" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <t>Name
 Enter a string.
@@ -805,12 +805,12 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Select a value from "Model:1" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Identifier
 Enter a string.
@@ -818,31 +818,31 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Name
 Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Select "True" or "False".</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
@@ -1149,28 +1149,28 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="2"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="5"/>
   <cols>
-    <col customWidth="1" max="3" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="4" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="3"/>
+    <col hidden="1" width="9" customWidth="1" min="4" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!!ObjTables ObjTablesVersion='0.0.8'</t>
+          <t>!!!ObjTables objTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='TableOfContents' Description='Table of contents' Date='2019-09-22 23:16:33' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='TableOfContents' description='Table of contents' date='2019-09-22 23:16:33' objTablesVersion='0.0.8'</t>
         </is>
       </c>
       <c r="B2" s="1" t="n"/>
@@ -1257,12 +1257,12 @@
   </sheetData>
   <autoFilter ref="A2:C6"/>
   <hyperlinks>
-    <hyperlink display="Schema" location="'!_Schema'!A1" ref="A3" tooltip="Click to view schema"/>
-    <hyperlink display="Compound" location="'!Compound'!A1" ref="A4" tooltip="Click to view compound"/>
-    <hyperlink display="Model" location="'!Model'!A1" ref="A5" tooltip="Click to view model"/>
-    <hyperlink display="Reaction" location="'!Reaction'!A1" ref="A6" tooltip="Click to view reaction"/>
+    <hyperlink ref="A3" location="'!_Schema'!A1" tooltip="Click to view schema" display="Schema"/>
+    <hyperlink ref="A4" location="'!Compound'!A1" tooltip="Click to view compound" display="Compound"/>
+    <hyperlink ref="A5" location="'!Model'!A1" tooltip="Click to view model" display="Model"/>
+    <hyperlink ref="A6" location="'!Reaction'!A1" tooltip="Click to view reaction" display="Reaction"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1275,21 +1275,21 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A5" ySplit="2"/>
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="7" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="8" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="7"/>
+    <col hidden="1" width="9" customWidth="1" min="8" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Schema' Description='Table/model and column/attribute definitions' Date='2019-09-22 23:16:33' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Schema' description='Table/model and column/attribute definitions' date='2019-09-22 23:16:33' objTablesVersion='0.0.8'</t>
         </is>
       </c>
       <c r="B1" s="1" t="n"/>
@@ -1812,11 +1812,11 @@
   </sheetData>
   <autoFilter ref="A2:G19"/>
   <hyperlinks>
-    <hyperlink display="Compound" location="'!Compound'!A1" ref="A3" tooltip="Click to view compound"/>
-    <hyperlink display="Model" location="'!Model'!A1" ref="A9" tooltip="Click to view model"/>
-    <hyperlink display="Reaction" location="'!Reaction'!A1" ref="A12" tooltip="Click to view reaction"/>
+    <hyperlink ref="A3" location="'!Compound'!A1" tooltip="Click to view compound" display="Compound"/>
+    <hyperlink ref="A9" location="'!Model'!A1" tooltip="Click to view model" display="Model"/>
+    <hyperlink ref="A12" location="'!Reaction'!A1" tooltip="Click to view reaction" display="Reaction"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1829,21 +1829,21 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="2"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="6"/>
   <cols>
-    <col customWidth="1" max="5" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="6" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="5"/>
+    <col hidden="1" width="9" customWidth="1" min="6" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Compound' Description='Compound' Name='Compound' Date='2019-09-22 23:16:33' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Compound' description='Compound' name='Compound' date='2019-09-22 23:16:33' objTablesVersion='0.0.8'</t>
         </is>
       </c>
       <c r="B1" s="1" t="n"/>
@@ -2006,24 +2006,24 @@
   </sheetData>
   <autoFilter ref="A2:E7"/>
   <dataValidations count="5">
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Identifiers" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="D3:D7" type="textLength">
+    <dataValidation sqref="D3:D7" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Identifiers" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be &quot;True&quot; or &quot;False&quot;." errorStyle="warning" errorTitle="IsConstant" prompt="Select &quot;True&quot; or &quot;False&quot;." promptTitle="IsConstant" showErrorMessage="1" showInputMessage="1" sqref="E3:E7" type="list">
+    <dataValidation sqref="E3:E7" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="IsConstant" error="Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="IsConstant" prompt="Select &quot;True&quot; or &quot;False&quot;." type="list" errorStyle="warning">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Identifier&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." errorStyle="warning" errorTitle="Id" operator="between" prompt="Identifier&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="B3:B7" type="textLength">
+    <dataValidation sqref="B3:B7" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Identifier&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Identifier&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Name&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Name&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="C3:C7" type="textLength">
+    <dataValidation sqref="C3:C7" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Name&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Name&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a value from &quot;Model:1&quot; or blank." errorStyle="warning" errorTitle="Model" prompt="Select a value from &quot;Model:1&quot; or blank." promptTitle="Model" showErrorMessage="1" showInputMessage="1" sqref="A3:A7" type="list">
+    <dataValidation sqref="A3:A7" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Model" error="Value must be a value from &quot;Model:1&quot; or blank." promptTitle="Model" prompt="Select a value from &quot;Model:1&quot; or blank." type="list" errorStyle="warning">
       <formula1>'[1]#REF'!$B$1:$XFD$1</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -2037,23 +2037,23 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="A2" pane="bottomRight" sqref="A2"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="2"/>
   <cols>
-    <col customWidth="1" max="2" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="3" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="2"/>
+    <col hidden="1" width="9" customWidth="1" min="3" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Model' Description='Model' Name='Model' Date='2019-09-22 23:16:33' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Model' description='Model' name='Model' date='2019-09-22 23:16:33' objTablesVersion='0.0.8'</t>
         </is>
       </c>
       <c r="B1" s="1" t="n"/>
@@ -2080,15 +2080,15 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="0" error="Name&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Name&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B3" type="textLength">
+    <dataValidation sqref="B3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Name&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Name&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Identifier&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." errorStyle="warning" errorTitle="Id" operator="between" prompt="Identifier&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="B2" type="textLength">
+    <dataValidation sqref="B2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Identifier&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Identifier&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -2102,21 +2102,21 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="2"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="3"/>
   <cols>
-    <col customWidth="1" max="7" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="8" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="7"/>
+    <col hidden="1" width="9" customWidth="1" min="8" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Reaction' Description='Reaction' Name='Reaction' Date='2019-09-22 23:16:33' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Reaction' description='Reaction' name='Reaction' date='2019-09-22 23:16:33' objTablesVersion='0.0.8'</t>
         </is>
       </c>
       <c r="B1" s="1" t="n"/>
@@ -2228,30 +2228,30 @@
   </sheetData>
   <autoFilter ref="A2:G4"/>
   <dataValidations count="7">
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Gene" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Gene" showErrorMessage="1" showInputMessage="1" sqref="G3:G4" type="textLength">
+    <dataValidation sqref="G3:G4" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Gene" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Gene" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be &quot;True&quot; or &quot;False&quot;." errorStyle="warning" errorTitle="IsReversible" prompt="Select &quot;True&quot; or &quot;False&quot;." promptTitle="IsReversible" showErrorMessage="1" showInputMessage="1" sqref="F3:F4" type="list">
+    <dataValidation sqref="F3:F4" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="IsReversible" error="Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="IsReversible" prompt="Select &quot;True&quot; or &quot;False&quot;." type="list" errorStyle="warning">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Equation" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Equation" showErrorMessage="1" showInputMessage="1" sqref="E3:E4" type="textLength">
+    <dataValidation sqref="E3:E4" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Equation" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Equation" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Identifiers" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="D3:D4" type="textLength">
+    <dataValidation sqref="D3:D4" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Identifiers" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Identifier&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." errorStyle="warning" errorTitle="Id" operator="between" prompt="Identifier&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="B3:B4" type="textLength">
+    <dataValidation sqref="B3:B4" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Identifier&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Identifier&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Name&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Name&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="C3:C4" type="textLength">
+    <dataValidation sqref="C3:C4" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Name&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Name&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a value from &quot;Model:1&quot; or blank." errorStyle="warning" errorTitle="Model" prompt="Select a value from &quot;Model:1&quot; or blank." promptTitle="Model" showErrorMessage="1" showInputMessage="1" sqref="A3:A4" type="list">
+    <dataValidation sqref="A3:A4" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Model" error="Value must be a value from &quot;Model:1&quot; or blank." promptTitle="Model" prompt="Select a value from &quot;Model:1&quot; or blank." type="list" errorStyle="warning">
       <formula1>'[1]#REF'!$B$1:$XFD$1</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>